<commit_message>
UserMeta toegevoegd en TagModel afgemaakt
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -38,6 +38,30 @@
   </si>
   <si>
     <t>1 uur</t>
+  </si>
+  <si>
+    <t>0,5 uur</t>
+  </si>
+  <si>
+    <t>Besproken wat er nog meer in ons NIAM schema moest komen te staan</t>
+  </si>
+  <si>
+    <t>2 uur</t>
+  </si>
+  <si>
+    <t>Een "GO" gekregen voor ons project</t>
+  </si>
+  <si>
+    <t>Groepsgesprek met Robert gehad</t>
+  </si>
+  <si>
+    <t>Bezig geweest met het uitwerken van de models</t>
+  </si>
+  <si>
+    <t>Video's gezien over ASP.NET</t>
+  </si>
+  <si>
+    <t>Models afgemaakt</t>
   </si>
 </sst>
 </file>
@@ -595,7 +619,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -695,7 +719,9 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
+      <c r="A5" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -706,14 +732,20 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
       <c r="K5" s="18"/>
-      <c r="L5" s="19"/>
+      <c r="L5" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="M5" s="20"/>
-      <c r="N5" s="21"/>
+      <c r="N5" s="37">
+        <v>40949</v>
+      </c>
       <c r="O5" s="22"/>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -724,14 +756,20 @@
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="18"/>
-      <c r="L6" s="19"/>
+      <c r="L6" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="M6" s="20"/>
-      <c r="N6" s="21"/>
+      <c r="N6" s="37">
+        <v>40953</v>
+      </c>
       <c r="O6" s="22"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -742,14 +780,20 @@
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
       <c r="K7" s="18"/>
-      <c r="L7" s="19"/>
+      <c r="L7" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="M7" s="20"/>
-      <c r="N7" s="21"/>
+      <c r="N7" s="37">
+        <v>40953</v>
+      </c>
       <c r="O7" s="22"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
+      <c r="A8" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -760,14 +804,20 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="19"/>
+      <c r="L8" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="M8" s="20"/>
-      <c r="N8" s="21"/>
+      <c r="N8" s="37">
+        <v>40955</v>
+      </c>
       <c r="O8" s="22"/>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -778,14 +828,20 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="18"/>
-      <c r="L9" s="19"/>
+      <c r="L9" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="M9" s="20"/>
-      <c r="N9" s="21"/>
+      <c r="N9" s="37">
+        <v>40961</v>
+      </c>
       <c r="O9" s="22"/>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -796,9 +852,13 @@
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="19"/>
+      <c r="L10" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="M10" s="20"/>
-      <c r="N10" s="21"/>
+      <c r="N10" s="37">
+        <v>40961</v>
+      </c>
       <c r="O10" s="22"/>
       <c r="P10" s="5"/>
     </row>

</xml_diff>

<commit_message>
Registratie gemaakt. (todo add succes page & confirm mail)
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>In en uitlog systeem gemaakt voor het project</t>
+  </si>
+  <si>
+    <t>Registratie systeem gemaakt</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -968,7 +971,9 @@
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
+      <c r="A15" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -979,9 +984,13 @@
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="19"/>
+      <c r="L15" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="M15" s="20"/>
-      <c r="N15" s="21"/>
+      <c r="N15" s="37">
+        <v>40975</v>
+      </c>
       <c r="O15" s="22"/>
       <c r="P15" s="5"/>
     </row>

</xml_diff>

<commit_message>
Activatie pagina toegevoegd. Mensen moeten nu eerst hun nieuwe account activeren voordat ze mogen. // Todo add mailer //
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Sidebar widget gemaakt voor de tags</t>
+  </si>
+  <si>
+    <t>Activatie pagina gemaakt waar mensen eerst moeten activeren voordat ze mogen inloggen</t>
   </si>
 </sst>
 </file>
@@ -634,7 +637,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1022,7 +1025,9 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
+      <c r="A17" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -1033,9 +1038,13 @@
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
       <c r="K17" s="18"/>
-      <c r="L17" s="19"/>
+      <c r="L17" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="M17" s="20"/>
-      <c r="N17" s="21"/>
+      <c r="N17" s="37">
+        <v>40976</v>
+      </c>
       <c r="O17" s="22"/>
       <c r="P17" s="5"/>
     </row>

</xml_diff>

<commit_message>
Wachtwoord vergeten afgemaakt + statische pagina's voor na het registreren en het veranderen van je wachtwoord (na wachtwoord vergeten).
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Detail view voor een question gemaakt</t>
+  </si>
+  <si>
+    <t>Statische pagina´s aangemaakt voor registreren en wachtwoord vergeten en het wachtwoord vergeten logica afgemaakt</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1076,7 +1079,9 @@
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
+      <c r="A19" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -1087,9 +1092,13 @@
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
       <c r="K19" s="18"/>
-      <c r="L19" s="19"/>
+      <c r="L19" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="M19" s="20"/>
-      <c r="N19" s="21"/>
+      <c r="N19" s="37">
+        <v>40980</v>
+      </c>
       <c r="O19" s="22"/>
       <c r="P19" s="5"/>
     </row>

</xml_diff>

<commit_message>
Profiel pagina home toegevoegd.
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>0,18 uur</t>
+  </si>
+  <si>
+    <t>Gewerkt aan account profiel pagina.</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1187,7 +1190,9 @@
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
+      <c r="A23" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -1198,9 +1203,13 @@
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="19"/>
+      <c r="L23" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="M23" s="20"/>
-      <c r="N23" s="21"/>
+      <c r="N23" s="37">
+        <v>40980</v>
+      </c>
       <c r="O23" s="22"/>
       <c r="P23" s="5"/>
     </row>

</xml_diff>

<commit_message>
Account instellingen pagina aangemaakt.
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -100,7 +100,10 @@
     <t>0,18 uur</t>
   </si>
   <si>
-    <t>Gewerkt aan account profiel pagina.</t>
+    <t>Account profiel pagina gemaakt.</t>
+  </si>
+  <si>
+    <t>Account instellingen pagina gemaakt.</t>
   </si>
 </sst>
 </file>
@@ -658,7 +661,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1208,13 +1211,15 @@
       </c>
       <c r="M23" s="20"/>
       <c r="N23" s="37">
-        <v>40980</v>
+        <v>40981</v>
       </c>
       <c r="O23" s="22"/>
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
+      <c r="A24" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -1225,9 +1230,13 @@
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="19"/>
+      <c r="L24" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="M24" s="20"/>
-      <c r="N24" s="21"/>
+      <c r="N24" s="37">
+        <v>40981</v>
+      </c>
       <c r="O24" s="22"/>
       <c r="P24" s="5"/>
     </row>

</xml_diff>

<commit_message>
Profiel overzichts pagina toegevoegd.
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Account instellingen pagina gemaakt.</t>
+  </si>
+  <si>
+    <t>Profiel pagina aangemaakt bij het klikken op een naam</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1241,7 +1244,9 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
+      <c r="A25" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -1252,9 +1257,13 @@
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
       <c r="K25" s="18"/>
-      <c r="L25" s="19"/>
+      <c r="L25" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="M25" s="20"/>
-      <c r="N25" s="21"/>
+      <c r="N25" s="37">
+        <v>40981</v>
+      </c>
       <c r="O25" s="22"/>
       <c r="P25" s="5"/>
     </row>

</xml_diff>

<commit_message>
Overzichtje geflaggde items gemaakt. (ToDo find a way to link comments and awnsers the right way, meaning to the correct item on the page)
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Profiel pagina aangemaakt bij het klikken op een naam</t>
+  </si>
+  <si>
+    <t>Admin overzichtje gemaakt van geflaggde comments/ antwoorden/ vrage</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1268,7 +1271,9 @@
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
+      <c r="A26" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -1279,9 +1284,13 @@
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="19"/>
+      <c r="L26" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="M26" s="20"/>
-      <c r="N26" s="21"/>
+      <c r="N26" s="37">
+        <v>40981</v>
+      </c>
       <c r="O26" s="22"/>
       <c r="P26" s="5"/>
     </row>

</xml_diff>

<commit_message>
Admin page verder gemaakt, mogelijk om nu comments te verwijderen die geflagged zijn
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>Admin overzichtje gemaakt van geflaggde comments/ antwoorden/ vrage</t>
+  </si>
+  <si>
+    <t>Admin overzichtje afgerond, nu mogelijk een comment te verwijderen</t>
+  </si>
+  <si>
+    <t>(totdat er een overzicht is van vraag + antwoorden en comments)</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -666,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U386"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1295,7 +1304,9 @@
       <c r="P26" s="5"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
+      <c r="A27" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -1306,15 +1317,21 @@
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
       <c r="K27" s="18"/>
-      <c r="L27" s="19"/>
+      <c r="L27" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="M27" s="20"/>
-      <c r="N27" s="21"/>
+      <c r="N27" s="37">
+        <v>40981</v>
+      </c>
       <c r="O27" s="22"/>
       <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -1324,9 +1341,13 @@
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
       <c r="K28" s="18"/>
-      <c r="L28" s="19"/>
+      <c r="L28" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="M28" s="20"/>
-      <c r="N28" s="21"/>
+      <c r="N28" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="O28" s="22"/>
       <c r="P28" s="5"/>
     </row>

</xml_diff>

<commit_message>
Stel een vraag begin opgebouwd
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>Bezig geweest met stel een vraag + controle of er niet al zo'n soort vraag bestaat</t>
+  </si>
+  <si>
+    <t>2,5 uur</t>
   </si>
 </sst>
 </file>
@@ -676,7 +682,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1328,7 @@
       </c>
       <c r="M27" s="20"/>
       <c r="N27" s="37">
-        <v>40981</v>
+        <v>40982</v>
       </c>
       <c r="O27" s="22"/>
       <c r="P27" s="5"/>
@@ -1352,7 +1358,9 @@
       <c r="P28" s="5"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
+      <c r="A29" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -1363,9 +1371,13 @@
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
       <c r="K29" s="18"/>
-      <c r="L29" s="19"/>
+      <c r="L29" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="M29" s="20"/>
-      <c r="N29" s="21"/>
+      <c r="N29" s="37">
+        <v>40953</v>
+      </c>
       <c r="O29" s="22"/>
       <c r="P29" s="5"/>
     </row>

</xml_diff>

<commit_message>
Stel een vraag toegevoegd + afgerond. En het aanmaken van user meta op het moment dat je registreerd :D
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>2,5 uur</t>
+  </si>
+  <si>
+    <t>Stel een vraag afgerond, werkt nu compleet</t>
+  </si>
+  <si>
+    <t>3,5 uur</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1382,7 +1388,9 @@
       <c r="P29" s="5"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
+      <c r="A30" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -1393,9 +1401,13 @@
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
       <c r="K30" s="18"/>
-      <c r="L30" s="19"/>
+      <c r="L30" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="M30" s="20"/>
-      <c r="N30" s="21"/>
+      <c r="N30" s="37">
+        <v>40983</v>
+      </c>
       <c r="O30" s="22"/>
       <c r="P30" s="5"/>
     </row>

</xml_diff>

<commit_message>
Pretified and debugged stel een vraag
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>3,5 uur</t>
+  </si>
+  <si>
+    <t>Steleen vraag netter gemaakt en een bug verholpen in stel een vraag</t>
   </si>
 </sst>
 </file>
@@ -688,7 +691,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1412,7 +1415,9 @@
       <c r="P30" s="5"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
+      <c r="A31" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -1423,9 +1428,13 @@
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="18"/>
-      <c r="L31" s="19"/>
+      <c r="L31" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="M31" s="20"/>
-      <c r="N31" s="21"/>
+      <c r="N31" s="37">
+        <v>40987</v>
+      </c>
       <c r="O31" s="22"/>
       <c r="P31" s="5"/>
     </row>

</xml_diff>

<commit_message>
Activeren + registreren af
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Vragen + antwoorden opnieuw toegevoegd</t>
+  </si>
+  <si>
+    <t>Mailer toegevoegd + een mail die gestuurd word op het moment dat je registreerd + activeerd</t>
   </si>
 </sst>
 </file>
@@ -697,7 +700,7 @@
   <dimension ref="A1:U386"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1496,9 @@
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
+      <c r="A34" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -1504,9 +1509,13 @@
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="19"/>
+      <c r="L34" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="M34" s="20"/>
-      <c r="N34" s="21"/>
+      <c r="N34" s="37">
+        <v>40959</v>
+      </c>
       <c r="O34" s="22"/>
       <c r="P34" s="5"/>
     </row>

</xml_diff>

<commit_message>
Alles omtrend mail gedaan.
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Mailer toegevoegd + een mail die gestuurd word op het moment dat je registreerd + activeerd</t>
+  </si>
+  <si>
+    <t>Mailer toegevoegd voor wachtwoord kwijt. Dit is nu ook af</t>
+  </si>
+  <si>
+    <t>0,2 uur</t>
   </si>
 </sst>
 </file>
@@ -699,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1449,7 +1455,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -1473,7 +1479,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -1490,14 +1496,14 @@
       </c>
       <c r="M33" s="20"/>
       <c r="N33" s="37">
-        <v>40959</v>
+        <v>40987</v>
       </c>
       <c r="O33" s="22"/>
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -1510,7 +1516,7 @@
       <c r="J34" s="17"/>
       <c r="K34" s="18"/>
       <c r="L34" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M34" s="20"/>
       <c r="N34" s="37">
@@ -1520,7 +1526,9 @@
       <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
+      <c r="A35" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -1531,14 +1539,20 @@
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="18"/>
-      <c r="L35" s="19"/>
+      <c r="L35" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="M35" s="20"/>
-      <c r="N35" s="21"/>
+      <c r="N35" s="37">
+        <v>40959</v>
+      </c>
       <c r="O35" s="22"/>
       <c r="P35" s="5"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
+      <c r="A36" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -1549,14 +1563,20 @@
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="19"/>
+      <c r="L36" s="19" t="s">
+        <v>4</v>
+      </c>
       <c r="M36" s="20"/>
-      <c r="N36" s="21"/>
+      <c r="N36" s="37">
+        <v>40988</v>
+      </c>
       <c r="O36" s="22"/>
       <c r="P36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
+      <c r="A37" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -1567,9 +1587,13 @@
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
       <c r="K37" s="18"/>
-      <c r="L37" s="19"/>
+      <c r="L37" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="M37" s="20"/>
-      <c r="N37" s="21"/>
+      <c r="N37" s="37">
+        <v>40988</v>
+      </c>
       <c r="O37" s="22"/>
       <c r="P37" s="5"/>
     </row>

</xml_diff>

<commit_message>
Admin panel af en een vraag beschikt over een delete knop (pretifie pls). Known bug: Bij vraag iets deleten maakt je header facked,moet nog naar gekeken worden.
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Deleten van een vraag toegevoegd</t>
+  </si>
+  <si>
+    <t>Deleten van een antwoord en een comment toegevoegd. Admin meuk is nu mogelijk af.</t>
   </si>
 </sst>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1679,7 +1682,9 @@
       <c r="P40" s="5"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
+      <c r="A41" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -1690,9 +1695,13 @@
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
       <c r="K41" s="18"/>
-      <c r="L41" s="19"/>
+      <c r="L41" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="M41" s="20"/>
-      <c r="N41" s="21"/>
+      <c r="N41" s="37">
+        <v>40995</v>
+      </c>
       <c r="O41" s="22"/>
       <c r="P41" s="5"/>
     </row>

</xml_diff>

<commit_message>
Mogelijkheid om alles te flaggen toegevoegd. Next up admin mass unflaggen en naar een antwoord of comment gaan vanuit beheer pagina.
</commit_message>
<xml_diff>
--- a/Logboeken/logboek Mathijs.xlsx
+++ b/Logboeken/logboek Mathijs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Mathijs Jonker</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Vote mogelijkheid toegevoegd</t>
+  </si>
+  <si>
+    <t>Mogelijkheid om een question, answer of een comment te flaggen toe gevoegd</t>
   </si>
 </sst>
 </file>
@@ -723,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1760,7 +1763,9 @@
       <c r="P43" s="5"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
+      <c r="A44" s="17" t="s">
+        <v>51</v>
+      </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
@@ -1771,9 +1776,13 @@
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
       <c r="K44" s="18"/>
-      <c r="L44" s="19"/>
+      <c r="L44" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="M44" s="20"/>
-      <c r="N44" s="21"/>
+      <c r="N44" s="37">
+        <v>40996</v>
+      </c>
       <c r="O44" s="22"/>
       <c r="P44" s="5"/>
     </row>

</xml_diff>